<commit_message>
ValueError 'Cannot convert A to excel '
</commit_message>
<xml_diff>
--- a/BeautifulSoup/Excel/Okky.xlsx
+++ b/BeautifulSoup/Excel/Okky.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:A321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,9 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-                크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위
-            </t>
+          <t>제목</t>
         </is>
       </c>
     </row>
@@ -434,7 +432,7 @@
       <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                (02/20) '패배자같은 개발 직무' 탈출법
+                크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위
             </t>
         </is>
       </c>
@@ -443,7 +441,7 @@
       <c r="A3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기
+                (02/20) '패배자같은 개발 직무' 탈출법
             </t>
         </is>
       </c>
@@ -452,7 +450,7 @@
       <c r="A4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                github 스카이라인
+                AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기
             </t>
         </is>
       </c>
@@ -461,7 +459,7 @@
       <c r="A5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                스프링 사이트(spring.io)를 로컬에서 실행하기
+                github 스카이라인
             </t>
         </is>
       </c>
@@ -470,7 +468,7 @@
       <c r="A6" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                spring boot 로컬에서 smtp mail 테스트하기
+                스프링 사이트(spring.io)를 로컬에서 실행하기
             </t>
         </is>
       </c>
@@ -479,7 +477,7 @@
       <c r="A7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                IoT디바이스를 위한 다양한 프레임워크/OS 소개!
+                spring boot 로컬에서 smtp mail 테스트하기
             </t>
         </is>
       </c>
@@ -488,7 +486,7 @@
       <c r="A8" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                [링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지
+                IoT디바이스를 위한 다양한 프레임워크/OS 소개!
             </t>
         </is>
       </c>
@@ -497,7 +495,7 @@
       <c r="A9" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력
+                [링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지
             </t>
         </is>
       </c>
@@ -506,7 +504,7 @@
       <c r="A10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                리액트 json으로 일부만 추출하기
+                Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력
             </t>
         </is>
       </c>
@@ -515,7 +513,7 @@
       <c r="A11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                Jenkins + Docker + AWS EC2 + Spring Boot
+                리액트 json으로 일부만 추출하기
             </t>
         </is>
       </c>
@@ -524,7 +522,7 @@
       <c r="A12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1
+                Jenkins + Docker + AWS EC2 + Spring Boot
             </t>
         </is>
       </c>
@@ -533,7 +531,7 @@
       <c r="A13" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                윤년인지 확인하는 JS
+                코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1
             </t>
         </is>
       </c>
@@ -542,7 +540,7 @@
       <c r="A14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                Bounded Context 어떻게 식별할 것 인가?
+                윤년인지 확인하는 JS
             </t>
         </is>
       </c>
@@ -551,7 +549,7 @@
       <c r="A15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                (02/13) 라인개발자들이 직접 뽑은 인생 책은?
+                Bounded Context 어떻게 식별할 것 인가?
             </t>
         </is>
       </c>
@@ -560,7 +558,7 @@
       <c r="A16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                maven central에 artifact 업로드
+                (02/13) 라인개발자들이 직접 뽑은 인생 책은?
             </t>
         </is>
       </c>
@@ -569,7 +567,7 @@
       <c r="A17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                깃헙 1초만에 VS Code로 보는 법
+                maven central에 artifact 업로드
             </t>
         </is>
       </c>
@@ -578,7 +576,7 @@
       <c r="A18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원
+                깃헙 1초만에 VS Code로 보는 법
             </t>
         </is>
       </c>
@@ -587,7 +585,7 @@
       <c r="A19" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                [iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선
+                개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원
             </t>
         </is>
       </c>
@@ -596,7 +594,7 @@
       <c r="A20" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수
+                [iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선
             </t>
         </is>
       </c>
@@ -605,7 +603,7 @@
       <c r="A21" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                스프링 부트에서 모든 메시지 코드 가져오기
+                프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수
             </t>
         </is>
       </c>
@@ -614,7 +612,7 @@
       <c r="A22" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                WebUtils.getNativeRequest 요청 래팽 해제
+                스프링 부트에서 모든 메시지 코드 가져오기
             </t>
         </is>
       </c>
@@ -623,7 +621,7 @@
       <c r="A23" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)
+                WebUtils.getNativeRequest 요청 래팽 해제
             </t>
         </is>
       </c>
@@ -632,7 +630,7 @@
       <c r="A24" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                DDD 아는 척 해보기
+                message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)
             </t>
         </is>
       </c>
@@ -641,7 +639,7 @@
       <c r="A25" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                도커 기초 명령어 #스프링부트
+                DDD 아는 척 해보기
             </t>
         </is>
       </c>
@@ -650,7 +648,7 @@
       <c r="A26" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것
+                도커 기초 명령어 #스프링부트
             </t>
         </is>
       </c>
@@ -659,7 +657,7 @@
       <c r="A27" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                logback 5분 마다 logfile 생성하기
+                7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것
             </t>
         </is>
       </c>
@@ -668,7 +666,7 @@
       <c r="A28" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                Garuda Linux
+                logback 5분 마다 logfile 생성하기
             </t>
         </is>
       </c>
@@ -677,7 +675,7 @@
       <c r="A29" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                MySQL 8.0 맥에 설치하기 #DBeaver
+                Garuda Linux
             </t>
         </is>
       </c>
@@ -686,7 +684,7 @@
       <c r="A30" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                스프링 부트 애플리케이션을 Vue와 함께 개발하기
+                MySQL 8.0 맥에 설치하기 #DBeaver
             </t>
         </is>
       </c>
@@ -695,7 +693,7 @@
       <c r="A31" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                tabulator VS dataTable 비교해본 결과
+                스프링 부트 애플리케이션을 Vue와 함께 개발하기
             </t>
         </is>
       </c>
@@ -704,7 +702,7 @@
       <c r="A32" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                spring에서 fcm (firebase cloud messaging) push 보내기.
+                tabulator VS dataTable 비교해본 결과
             </t>
         </is>
       </c>
@@ -713,7 +711,7 @@
       <c r="A33" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                DD-Sketch 소개
+                spring에서 fcm (firebase cloud messaging) push 보내기.
             </t>
         </is>
       </c>
@@ -722,7 +720,7 @@
       <c r="A34" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                Software Design 역사로 이해하는 DDD
+                DD-Sketch 소개
             </t>
         </is>
       </c>
@@ -731,7 +729,7 @@
       <c r="A35" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                리눅스 배포판 선택을 도와주는 서비스
+                Software Design 역사로 이해하는 DDD
             </t>
         </is>
       </c>
@@ -740,7 +738,7 @@
       <c r="A36" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                (01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?
+                리눅스 배포판 선택을 도와주는 서비스
             </t>
         </is>
       </c>
@@ -749,7 +747,7 @@
       <c r="A37" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                [영상] 스프링 부트 MyBatis
+                (01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?
             </t>
         </is>
       </c>
@@ -758,7 +756,7 @@
       <c r="A38" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                TOAST UI Chart 4.0이 출시되었습니다.
+                [영상] 스프링 부트 MyBatis
             </t>
         </is>
       </c>
@@ -767,7 +765,7 @@
       <c r="A39" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                JWT Token를 spring security에서 손쉽게 검증하기 위한 방법
+                TOAST UI Chart 4.0이 출시되었습니다.
             </t>
         </is>
       </c>
@@ -776,7 +774,7 @@
       <c r="A40" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"
+                JWT Token를 spring security에서 손쉽게 검증하기 위한 방법
             </t>
         </is>
       </c>
@@ -785,7 +783,7 @@
       <c r="A41" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                Software Architecture 역사로 이해하는 MSA
+                페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"
             </t>
         </is>
       </c>
@@ -794,7 +792,7 @@
       <c r="A42" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                [JS] 한글도 지원하는 퍼지 문자열 검색
+                Software Architecture 역사로 이해하는 MSA
             </t>
         </is>
       </c>
@@ -803,7 +801,7 @@
       <c r="A43" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                애플에서 한국에 코딩 아카데미 설립한다고 하네요
+                [JS] 한글도 지원하는 퍼지 문자열 검색
             </t>
         </is>
       </c>
@@ -812,7 +810,7 @@
       <c r="A44" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                테크 뉴스를 편하게 보는 방법
+                애플에서 한국에 코딩 아카데미 설립한다고 하네요
             </t>
         </is>
       </c>
@@ -821,7 +819,7 @@
       <c r="A45" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                (01/22) 프론트엔드 성능 점검 항목 – 2021 버전
+                테크 뉴스를 편하게 보는 방법
             </t>
         </is>
       </c>
@@ -830,7 +828,7 @@
       <c r="A46" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                React 불필요한 렌더링을 막는 방법
+                (01/22) 프론트엔드 성능 점검 항목 – 2021 버전
             </t>
         </is>
       </c>
@@ -839,7 +837,7 @@
       <c r="A47" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                라즈베리파이, 아두이노 경쟁작 '피코' 출시
+                React 불필요한 렌더링을 막는 방법
             </t>
         </is>
       </c>
@@ -848,7 +846,7 @@
       <c r="A48" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                최근 Elasticsearch 유료화 이슈 대응
+                라즈베리파이, 아두이노 경쟁작 '피코' 출시
             </t>
         </is>
       </c>
@@ -857,7 +855,7 @@
       <c r="A49" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                가상화 및 하이퍼바이저 간단 개념 소개.
+                최근 Elasticsearch 유료화 이슈 대응
             </t>
         </is>
       </c>
@@ -866,7 +864,7 @@
       <c r="A50" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                삼성 엑시노스 컴퓨터 나오나?
+                가상화 및 하이퍼바이저 간단 개념 소개.
             </t>
         </is>
       </c>
@@ -875,7 +873,7 @@
       <c r="A51" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                MSA 도입 평가 체크리스트
+                삼성 엑시노스 컴퓨터 나오나?
             </t>
         </is>
       </c>
@@ -884,7 +882,7 @@
       <c r="A52" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                스프링 부트 DB 트랜잭션
+                MSA 도입 평가 체크리스트
             </t>
         </is>
       </c>
@@ -893,7 +891,7 @@
       <c r="A53" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                태블릿 기반의 리눅스 배포판 - JingOS
+                스프링 부트 DB 트랜잭션
             </t>
         </is>
       </c>
@@ -902,7 +900,7 @@
       <c r="A54" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                스프링 부트 자동 재시작 설정하기 #개발모드
+                태블릿 기반의 리눅스 배포판 - JingOS
             </t>
         </is>
       </c>
@@ -911,7 +909,7 @@
       <c r="A55" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                State of js 2020: 프론트엔드 프레임워크 이야기
+                스프링 부트 자동 재시작 설정하기 #개발모드
             </t>
         </is>
       </c>
@@ -920,7 +918,7 @@
       <c r="A56" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                메일 서버와 스팸 서버 구축
+                State of js 2020: 프론트엔드 프레임워크 이야기
             </t>
         </is>
       </c>
@@ -929,7 +927,7 @@
       <c r="A57" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                2020 떠오른 자바스크립트 프로젝트 랭킹
+                메일 서버와 스팸 서버 구축
             </t>
         </is>
       </c>
@@ -938,7 +936,7 @@
       <c r="A58" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                무제한 무료 프론트엔드 코드 저장소
+                2020 떠오른 자바스크립트 프로젝트 랭킹
             </t>
         </is>
       </c>
@@ -947,7 +945,7 @@
       <c r="A59" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                (01/16) 마이크로서비스 도입, 이렇게 한다
+                무제한 무료 프론트엔드 코드 저장소
             </t>
         </is>
       </c>
@@ -956,8 +954,1957 @@
       <c r="A60" t="inlineStr">
         <is>
           <t xml:space="preserve">
+                (01/16) 마이크로서비스 도입, 이렇게 한다
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
                 JPA 연관 관계를 명시(사용)하는 이유는 무엇일까?(불일치패러다임설명하는 글이 아닙니다...)
             </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>(02/20) '패배자같은 개발 직무' 탈출법</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>github 스카이라인</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>스프링 사이트(spring.io)를 로컬에서 실행하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>spring boot 로컬에서 smtp mail 테스트하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>IoT디바이스를 위한 다양한 프레임워크/OS 소개!</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>[링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>리액트 json으로 일부만 추출하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Jenkins + Docker + AWS EC2 + Spring Boot</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>윤년인지 확인하는 JS</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Bounded Context 어떻게 식별할 것 인가?</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>(02/13) 라인개발자들이 직접 뽑은 인생 책은?</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>maven central에 artifact 업로드</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>깃헙 1초만에 VS Code로 보는 법</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>[iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>스프링 부트에서 모든 메시지 코드 가져오기</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>WebUtils.getNativeRequest 요청 래팽 해제</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>DDD 아는 척 해보기</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>도커 기초 명령어 #스프링부트</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>logback 5분 마다 logfile 생성하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Garuda Linux</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>MySQL 8.0 맥에 설치하기 #DBeaver</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>스프링 부트 애플리케이션을 Vue와 함께 개발하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>tabulator VS dataTable 비교해본 결과</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>spring에서 fcm (firebase cloud messaging) push 보내기.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>DD-Sketch 소개</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Software Design 역사로 이해하는 DDD</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>리눅스 배포판 선택을 도와주는 서비스</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>(01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>[영상] 스프링 부트 MyBatis</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>TOAST UI Chart 4.0이 출시되었습니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>JWT Token를 spring security에서 손쉽게 검증하기 위한 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Software Architecture 역사로 이해하는 MSA</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>[JS] 한글도 지원하는 퍼지 문자열 검색</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>애플에서 한국에 코딩 아카데미 설립한다고 하네요</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>테크 뉴스를 편하게 보는 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>(01/22) 프론트엔드 성능 점검 항목 – 2021 버전</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>React 불필요한 렌더링을 막는 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>라즈베리파이, 아두이노 경쟁작 '피코' 출시</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>최근 Elasticsearch 유료화 이슈 대응</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>가상화 및 하이퍼바이저 간단 개념 소개.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>삼성 엑시노스 컴퓨터 나오나?</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>MSA 도입 평가 체크리스트</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>스프링 부트 DB 트랜잭션</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>태블릿 기반의 리눅스 배포판 - JingOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>스프링 부트 자동 재시작 설정하기 #개발모드</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>State of js 2020: 프론트엔드 프레임워크 이야기</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>메일 서버와 스팸 서버 구축</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2020 떠오른 자바스크립트 프로젝트 랭킹</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>무제한 무료 프론트엔드 코드 저장소</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>(01/16) 마이크로서비스 도입, 이렇게 한다</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>JPA 연관 관계를 명시(사용)하는 이유는 무엇일까?(불일치패러다임설명하는 글이 아닙니다...)</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                (02/20) '패배자같은 개발 직무' 탈출법
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                github 스카이라인
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                스프링 사이트(spring.io)를 로컬에서 실행하기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                spring boot 로컬에서 smtp mail 테스트하기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                IoT디바이스를 위한 다양한 프레임워크/OS 소개!
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                [링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                리액트 json으로 일부만 추출하기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                Jenkins + Docker + AWS EC2 + Spring Boot
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                윤년인지 확인하는 JS
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                Bounded Context 어떻게 식별할 것 인가?
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                (02/13) 라인개발자들이 직접 뽑은 인생 책은?
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                maven central에 artifact 업로드
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                깃헙 1초만에 VS Code로 보는 법
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                [iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                스프링 부트에서 모든 메시지 코드 가져오기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                WebUtils.getNativeRequest 요청 래팽 해제
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                DDD 아는 척 해보기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                도커 기초 명령어 #스프링부트
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                logback 5분 마다 logfile 생성하기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                Garuda Linux
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                MySQL 8.0 맥에 설치하기 #DBeaver
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                스프링 부트 애플리케이션을 Vue와 함께 개발하기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                tabulator VS dataTable 비교해본 결과
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                spring에서 fcm (firebase cloud messaging) push 보내기.
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                DD-Sketch 소개
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                Software Design 역사로 이해하는 DDD
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                리눅스 배포판 선택을 도와주는 서비스
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                (01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                [영상] 스프링 부트 MyBatis
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                TOAST UI Chart 4.0이 출시되었습니다.
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                JWT Token를 spring security에서 손쉽게 검증하기 위한 방법
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                Software Architecture 역사로 이해하는 MSA
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                [JS] 한글도 지원하는 퍼지 문자열 검색
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                애플에서 한국에 코딩 아카데미 설립한다고 하네요
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                테크 뉴스를 편하게 보는 방법
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                (01/22) 프론트엔드 성능 점검 항목 – 2021 버전
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                React 불필요한 렌더링을 막는 방법
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                라즈베리파이, 아두이노 경쟁작 '피코' 출시
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                최근 Elasticsearch 유료화 이슈 대응
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                가상화 및 하이퍼바이저 간단 개념 소개.
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                삼성 엑시노스 컴퓨터 나오나?
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                MSA 도입 평가 체크리스트
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                스프링 부트 DB 트랜잭션
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                태블릿 기반의 리눅스 배포판 - JingOS
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                스프링 부트 자동 재시작 설정하기 #개발모드
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                State of js 2020: 프론트엔드 프레임워크 이야기
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                메일 서버와 스팸 서버 구축
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                2020 떠오른 자바스크립트 프로젝트 랭킹
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                무제한 무료 프론트엔드 코드 저장소
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                (01/16) 마이크로서비스 도입, 이렇게 한다
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                JPA 연관 관계를 명시(사용)하는 이유는 무엇일까?(불일치패러다임설명하는 글이 아닙니다...)
+            </t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>(02/20) '패배자같은 개발 직무' 탈출법</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>github 스카이라인</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>스프링 사이트(spring.io)를 로컬에서 실행하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>spring boot 로컬에서 smtp mail 테스트하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>IoT디바이스를 위한 다양한 프레임워크/OS 소개!</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>[링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>리액트 json으로 일부만 추출하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Jenkins + Docker + AWS EC2 + Spring Boot</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>윤년인지 확인하는 JS</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Bounded Context 어떻게 식별할 것 인가?</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>(02/13) 라인개발자들이 직접 뽑은 인생 책은?</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>maven central에 artifact 업로드</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>깃헙 1초만에 VS Code로 보는 법</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>[iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>스프링 부트에서 모든 메시지 코드 가져오기</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>WebUtils.getNativeRequest 요청 래팽 해제</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>DDD 아는 척 해보기</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>도커 기초 명령어 #스프링부트</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>logback 5분 마다 logfile 생성하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Garuda Linux</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>MySQL 8.0 맥에 설치하기 #DBeaver</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>스프링 부트 애플리케이션을 Vue와 함께 개발하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>tabulator VS dataTable 비교해본 결과</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>spring에서 fcm (firebase cloud messaging) push 보내기.</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>DD-Sketch 소개</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Software Design 역사로 이해하는 DDD</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>리눅스 배포판 선택을 도와주는 서비스</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>(01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>[영상] 스프링 부트 MyBatis</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>TOAST UI Chart 4.0이 출시되었습니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>JWT Token를 spring security에서 손쉽게 검증하기 위한 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Software Architecture 역사로 이해하는 MSA</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>[JS] 한글도 지원하는 퍼지 문자열 검색</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>애플에서 한국에 코딩 아카데미 설립한다고 하네요</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>테크 뉴스를 편하게 보는 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>(01/22) 프론트엔드 성능 점검 항목 – 2021 버전</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>React 불필요한 렌더링을 막는 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>라즈베리파이, 아두이노 경쟁작 '피코' 출시</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>최근 Elasticsearch 유료화 이슈 대응</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>가상화 및 하이퍼바이저 간단 개념 소개.</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>삼성 엑시노스 컴퓨터 나오나?</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>MSA 도입 평가 체크리스트</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>스프링 부트 DB 트랜잭션</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>태블릿 기반의 리눅스 배포판 - JingOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>스프링 부트 자동 재시작 설정하기 #개발모드</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>State of js 2020: 프론트엔드 프레임워크 이야기</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>메일 서버와 스팸 서버 구축</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2020 떠오른 자바스크립트 프로젝트 랭킹</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>무제한 무료 프론트엔드 코드 저장소</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>(01/16) 마이크로서비스 도입, 이렇게 한다</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>JPA 연관 관계를 명시(사용)하는 이유는 무엇일까?(불일치패러다임설명하는 글이 아닙니다...)</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>(02/20) '패배자같은 개발 직무' 탈출법</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>github 스카이라인</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>스프링 사이트(spring.io)를 로컬에서 실행하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>spring boot 로컬에서 smtp mail 테스트하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>IoT디바이스를 위한 다양한 프레임워크/OS 소개!</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>[링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>리액트 json으로 일부만 추출하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Jenkins + Docker + AWS EC2 + Spring Boot</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>윤년인지 확인하는 JS</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Bounded Context 어떻게 식별할 것 인가?</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>(02/13) 라인개발자들이 직접 뽑은 인생 책은?</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>maven central에 artifact 업로드</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>깃헙 1초만에 VS Code로 보는 법</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>[iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>스프링 부트에서 모든 메시지 코드 가져오기</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>WebUtils.getNativeRequest 요청 래팽 해제</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>DDD 아는 척 해보기</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>도커 기초 명령어 #스프링부트</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>logback 5분 마다 logfile 생성하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Garuda Linux</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>MySQL 8.0 맥에 설치하기 #DBeaver</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>스프링 부트 애플리케이션을 Vue와 함께 개발하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>tabulator VS dataTable 비교해본 결과</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>spring에서 fcm (firebase cloud messaging) push 보내기.</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>DD-Sketch 소개</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Software Design 역사로 이해하는 DDD</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>리눅스 배포판 선택을 도와주는 서비스</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>(01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>[영상] 스프링 부트 MyBatis</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>TOAST UI Chart 4.0이 출시되었습니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>JWT Token를 spring security에서 손쉽게 검증하기 위한 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>크롬OS, 맥OS 제쳤다....PC용 OS 점유율 2위</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>(02/20) '패배자같은 개발 직무' 탈출법</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>AWS 시스템 매니저로 관리형 EC2 인스턴스에 연결하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>github 스카이라인</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>스프링 사이트(spring.io)를 로컬에서 실행하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>spring boot 로컬에서 smtp mail 테스트하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>IoT디바이스를 위한 다양한 프레임워크/OS 소개!</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>[링크] 개발자가 처음 Docker 접할때 오는 멘붕 몇가지</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Noticon 프로젝트 리뷰 - 돈 한 푼 안들이고 서비스를 운영하기 위한 노력</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>리액트 json으로 일부만 추출하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Jenkins + Docker + AWS EC2 + Spring Boot</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>코딩 플레이그라운드 만들며 맛보는 요즘 FE 개발 환경 Part 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>윤년인지 확인하는 JS</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Bounded Context 어떻게 식별할 것 인가?</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>(02/13) 라인개발자들이 직접 뽑은 인생 책은?</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>maven central에 artifact 업로드</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>깃헙 1초만에 VS Code로 보는 법</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>개발언어 Rust 가 Rust 재단으로 독립 / AWS, 화웨이, 구글, 마소, 모질라에서 지원</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>[iOS] WKWebView에서 Native &lt;-&gt; Javascript간 Communication개선</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>프로그램 소스에 비번, API키 등의 하드코딩 피하는 법 #환경변수</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>스프링 부트에서 모든 메시지 코드 가져오기</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>WebUtils.getNativeRequest 요청 래팽 해제</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>message.properties → *.json 변환하여 프론트 프로젝트에 넣기. (gradle)</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>DDD 아는 척 해보기</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>도커 기초 명령어 #스프링부트</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>7년 차 SI 개발자가 솔루션 회사 이직 후 2년 간 배운 것</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>logback 5분 마다 logfile 생성하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Garuda Linux</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>MySQL 8.0 맥에 설치하기 #DBeaver</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>스프링 부트 애플리케이션을 Vue와 함께 개발하기</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>tabulator VS dataTable 비교해본 결과</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>spring에서 fcm (firebase cloud messaging) push 보내기.</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>DD-Sketch 소개</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Software Design 역사로 이해하는 DDD</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>리눅스 배포판 선택을 도와주는 서비스</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>(01/30) 정말로 당신에게 다른 동영상 강의가 필요할까?</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>[영상] 스프링 부트 MyBatis</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>TOAST UI Chart 4.0이 출시되었습니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>JWT Token를 spring security에서 손쉽게 검증하기 위한 방법</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>페도라 OS 브라우저 책임자 "크롬 대신 파이어폭스 써라"</t>
         </is>
       </c>
     </row>

</xml_diff>